<commit_message>
hide controls at first load
</commit_message>
<xml_diff>
--- a/002 Javascript, Jquery and Angular - UI Guidelines.xlsx
+++ b/002 Javascript, Jquery and Angular - UI Guidelines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\ws\iihtibm-angular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A5FF725-A142-4290-9D1C-36BC9CE02206}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712F8634-CB57-4245-AECD-36A3D1AC3BBA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" activeTab="1" xr2:uid="{CDD88839-9D49-488E-BB39-C9224342197E}"/>
   </bookViews>
@@ -6630,8 +6630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B57575-EDC9-4C52-9F23-3DC304D1C029}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C31" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6815,7 +6815,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -6827,7 +6827,7 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>17</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>